<commit_message>
Completed class 8 workshop
</commit_message>
<xml_diff>
--- a/Random.xlsx
+++ b/Random.xlsx
@@ -14,22 +14,22 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>Elenor</t>
+    <t>Pat</t>
   </si>
   <si>
-    <t>869</t>
+    <t>89067</t>
   </si>
   <si>
-    <t>1-961-618-3091 x9043</t>
+    <t>1-027-368-7432</t>
   </si>
   <si>
-    <t>Cristobal</t>
+    <t>Therese</t>
   </si>
   <si>
-    <t>4243</t>
+    <t>1912</t>
   </si>
   <si>
-    <t>366-039-8606 x66292</t>
+    <t>1-124-506-6318 x44184</t>
   </si>
 </sst>
 </file>

</xml_diff>